<commit_message>
comparison momentum error and energy error
for the inviscid shear layer test case
</commit_message>
<xml_diff>
--- a/results/testcase_list.xlsx
+++ b/results/testcase_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanderse/Dropbox/work/Programming/INS/2D/INS2D/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E96FDF-D39C-CA4E-AF85-4B50CD828EC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCCEB98-0AED-874F-96AD-0A5C8B3857D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="10020" windowWidth="34820" windowHeight="21740" xr2:uid="{CC858DF3-E617-C248-857C-D84B31F2A343}"/>
+    <workbookView xWindow="12020" yWindow="5600" windowWidth="34820" windowHeight="21740" xr2:uid="{CC858DF3-E617-C248-857C-D84B31F2A343}"/>
   </bookViews>
   <sheets>
     <sheet name="shear layer" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>shear_layer_1.000e+02_6.2832x6.2832_200x200_FOM</t>
-  </si>
-  <si>
     <t>200x200</t>
   </si>
   <si>
@@ -81,10 +78,46 @@
     <t>RK44</t>
   </si>
   <si>
-    <t>shear_layer_1.000e+100_6.2832x6.2832_40x40_momcons_FOM</t>
-  </si>
-  <si>
     <t>40x40</t>
+  </si>
+  <si>
+    <t>shear_layer01</t>
+  </si>
+  <si>
+    <t>Initial condition</t>
+  </si>
+  <si>
+    <t>shear layer + 1 for u comp</t>
+  </si>
+  <si>
+    <t>shear layer standard</t>
+  </si>
+  <si>
+    <t>shear_layer02</t>
+  </si>
+  <si>
+    <t>shear_layer03</t>
+  </si>
+  <si>
+    <t>GL1</t>
+  </si>
+  <si>
+    <t>ROM</t>
+  </si>
+  <si>
+    <t>shear_layer01/matlab_data.mat</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>not momentum conserving</t>
+  </si>
+  <si>
+    <t>2,4,8,16</t>
+  </si>
+  <si>
+    <t>momentum conserving</t>
   </si>
 </sst>
 </file>
@@ -138,6 +171,29 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D671E48-07DB-A240-B7CB-2166D3ACE288}" name="Table1" displayName="Table1" ref="A3:N8" totalsRowShown="0">
+  <autoFilter ref="A3:N8" xr:uid="{D2B70914-856C-5A42-8F2C-FDB5ECFC523E}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{AA1E7D86-BA4C-DC45-92FB-170CBEEF8D4B}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{477827BE-4E67-A048-8047-07DAFF7AC5BF}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{B9EF05BD-385F-374A-AC1A-C5831A8620A7}" name="Figure in report"/>
+    <tableColumn id="4" xr3:uid="{AAA4DA3A-1671-C64B-8733-00573B024311}" name="Initial condition"/>
+    <tableColumn id="5" xr3:uid="{D8516B90-E3F3-924E-821E-CDBE977DF5DD}" name="Reynolds number"/>
+    <tableColumn id="6" xr3:uid="{51FBA729-CA38-E945-838C-465E445C3A1E}" name="Volumes"/>
+    <tableColumn id="7" xr3:uid="{BF87B10A-9F63-A34A-A3E1-C9F6EECF844F}" name="boundary conditions"/>
+    <tableColumn id="8" xr3:uid="{98D61AC5-6CD7-9C49-AEF6-3A57D91FBAB6}" name="dt"/>
+    <tableColumn id="9" xr3:uid="{64CF17BF-0318-D341-B0FA-30F66B73694A}" name="t_end"/>
+    <tableColumn id="10" xr3:uid="{A410EBBD-CD18-6543-8167-7B77459FFA83}" name="time integration method"/>
+    <tableColumn id="11" xr3:uid="{DC4923B7-E855-D348-AEE0-D2DB19B3B678}" name="FOM / ROM"/>
+    <tableColumn id="12" xr3:uid="{8B8E3D4C-7AA0-E94C-AC34-662D0FC7D3BB}" name="# modes of ROM"/>
+    <tableColumn id="13" xr3:uid="{00A4BD27-AB66-B143-8890-4E19CAE373BA}" name="snapshot matrix file"/>
+    <tableColumn id="14" xr3:uid="{7AACCEED-6AFF-A04A-B090-C308F10F13E2}" name="Other"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,27 +493,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E178FB4-9DEC-9D41-B392-EF840F186371}">
-  <dimension ref="A3:L5"/>
+  <dimension ref="A3:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="55.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
-    <col min="11" max="11" width="20.1640625" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -465,89 +521,218 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1E+100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1E+100</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1E+100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1E+100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1E+100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1E+100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4">
+      <c r="I8">
         <v>4</v>
       </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1E+100</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>11</v>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
non-homogeneous BC for ROM
* added non-homogeneous BC capability for ROM
* solves Poisson equation to get BC contribution, which is subtracted from snapshot matrix
* both explicit and implicit time integration have been tested
</commit_message>
<xml_diff>
--- a/results/testcase_list.xlsx
+++ b/results/testcase_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanderse/Dropbox/work/Programming/INS/2D/INS2D/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA09EB9-51D1-B648-88EF-97A7BA65F07F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3DB456-8DED-DF4D-8B9B-7881FD8564C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16660" yWindow="12040" windowWidth="34820" windowHeight="21740" xr2:uid="{CC858DF3-E617-C248-857C-D84B31F2A343}"/>
+    <workbookView xWindow="1540" yWindow="10300" windowWidth="34820" windowHeight="21740" xr2:uid="{CC858DF3-E617-C248-857C-D84B31F2A343}"/>
   </bookViews>
   <sheets>
     <sheet name="shear layer" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -142,6 +142,27 @@
   </si>
   <si>
     <t>actuator_unsteady01/matlab_data.mat</t>
+  </si>
+  <si>
+    <t>actuator_unsteady02</t>
+  </si>
+  <si>
+    <t>not mass conserving</t>
+  </si>
+  <si>
+    <t>actuator_unsteady03</t>
+  </si>
+  <si>
+    <t>mass conserving</t>
+  </si>
+  <si>
+    <t>actuator_unsteady04</t>
+  </si>
+  <si>
+    <t>movie</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -198,9 +219,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D671E48-07DB-A240-B7CB-2166D3ACE288}" name="Table1" displayName="Table1" ref="A3:N9" totalsRowShown="0">
-  <autoFilter ref="A3:N9" xr:uid="{D2B70914-856C-5A42-8F2C-FDB5ECFC523E}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D671E48-07DB-A240-B7CB-2166D3ACE288}" name="Table1" displayName="Table1" ref="A3:O11" totalsRowShown="0">
+  <autoFilter ref="A3:O11" xr:uid="{D2B70914-856C-5A42-8F2C-FDB5ECFC523E}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{AA1E7D86-BA4C-DC45-92FB-170CBEEF8D4B}" name="ID"/>
     <tableColumn id="2" xr3:uid="{477827BE-4E67-A048-8047-07DAFF7AC5BF}" name="Name"/>
     <tableColumn id="3" xr3:uid="{B9EF05BD-385F-374A-AC1A-C5831A8620A7}" name="Figure in report"/>
@@ -214,6 +235,7 @@
     <tableColumn id="11" xr3:uid="{DC4923B7-E855-D348-AEE0-D2DB19B3B678}" name="FOM / ROM"/>
     <tableColumn id="12" xr3:uid="{8B8E3D4C-7AA0-E94C-AC34-662D0FC7D3BB}" name="# modes of ROM"/>
     <tableColumn id="13" xr3:uid="{00A4BD27-AB66-B143-8890-4E19CAE373BA}" name="snapshot matrix file"/>
+    <tableColumn id="15" xr3:uid="{14F49858-CE70-D54E-9D2A-B3C51E7BC909}" name="movie"/>
     <tableColumn id="14" xr3:uid="{7AACCEED-6AFF-A04A-B090-C308F10F13E2}" name="Other"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -517,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E178FB4-9DEC-9D41-B392-EF840F186371}">
-  <dimension ref="A3:N9"/>
+  <dimension ref="A3:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,11 +556,12 @@
     <col min="10" max="10" width="23.6640625" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="30" customWidth="1"/>
-    <col min="14" max="14" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30" customWidth="1"/>
+    <col min="15" max="15" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -579,10 +602,13 @@
         <v>13</v>
       </c>
       <c r="N3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -614,7 +640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -646,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -678,7 +704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -715,11 +741,11 @@
       <c r="M7" t="s">
         <v>26</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -756,11 +782,11 @@
       <c r="M8" t="s">
         <v>26</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -791,8 +817,134 @@
       <c r="K9" t="s">
         <v>10</v>
       </c>
-      <c r="M9" t="s">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10" t="s">
         <v>38</v>
+      </c>
+      <c r="O10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actuator test case with parabolic inflow
settings to generate FOM results
</commit_message>
<xml_diff>
--- a/results/testcase_list.xlsx
+++ b/results/testcase_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanderse/Dropbox/work/Programming/INS/2D/INS2D/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3DB456-8DED-DF4D-8B9B-7881FD8564C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D823953B-0AB1-1C4C-B62F-41533933730F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="10300" windowWidth="34820" windowHeight="21740" xr2:uid="{CC858DF3-E617-C248-857C-D84B31F2A343}"/>
+    <workbookView xWindow="2040" yWindow="5960" windowWidth="46020" windowHeight="22760" xr2:uid="{CC858DF3-E617-C248-857C-D84B31F2A343}"/>
   </bookViews>
   <sheets>
     <sheet name="shear layer" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>actuator_unsteady05</t>
+  </si>
+  <si>
+    <t>u=parabolic</t>
   </si>
 </sst>
 </file>
@@ -178,15 +184,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -194,13 +206,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,8 +242,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D671E48-07DB-A240-B7CB-2166D3ACE288}" name="Table1" displayName="Table1" ref="A3:O11" totalsRowShown="0">
-  <autoFilter ref="A3:O11" xr:uid="{D2B70914-856C-5A42-8F2C-FDB5ECFC523E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D671E48-07DB-A240-B7CB-2166D3ACE288}" name="Table1" displayName="Table1" ref="A3:O14" totalsRowShown="0">
+  <autoFilter ref="A3:O14" xr:uid="{D2B70914-856C-5A42-8F2C-FDB5ECFC523E}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{AA1E7D86-BA4C-DC45-92FB-170CBEEF8D4B}" name="ID"/>
     <tableColumn id="2" xr3:uid="{477827BE-4E67-A048-8047-07DAFF7AC5BF}" name="Name"/>
@@ -539,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E178FB4-9DEC-9D41-B392-EF840F186371}">
-  <dimension ref="A3:O12"/>
+  <dimension ref="A3:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -947,6 +970,48 @@
         <v>42</v>
       </c>
     </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="2">
+        <v>100</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="3">
+        <v>10</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added discrete fourier transform as pressure solver
- for periodic boundary conditions and uniform grids
- tested on TG testcase
- see pressure_poisson and operator_divergence
</commit_message>
<xml_diff>
--- a/results/testcase_list.xlsx
+++ b/results/testcase_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanderse/Dropbox/work/Programming/INS/2D/INS2D/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86449219-D676-3F4B-B1B5-D3A69938B352}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F542DC-571D-604B-855F-19DBAAC401D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="4500" windowWidth="46020" windowHeight="22760" xr2:uid="{CC858DF3-E617-C248-857C-D84B31F2A343}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" xr2:uid="{CC858DF3-E617-C248-857C-D84B31F2A343}"/>
   </bookViews>
   <sheets>
     <sheet name="shear layer" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>not energy-conserving yet; need change of norm</t>
+  </si>
+  <si>
+    <t>shear_layer_ROM_snapshots_rerunApril2020</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="C7" sqref="C7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,6 +978,14 @@
       </c>
       <c r="P11" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>